<commit_message>
More task status related stuff
</commit_message>
<xml_diff>
--- a/data/task_status.xlsx
+++ b/data/task_status.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t xml:space="preserve">task</t>
   </si>
@@ -44,6 +44,27 @@
   </si>
   <si>
     <t xml:space="preserve">67_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNF_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNF_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNF_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNF_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">893422_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">893422_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNF_7</t>
   </si>
 </sst>
 </file>
@@ -53,11 +74,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -73,6 +95,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,9 +146,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -245,51 +282,107 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed spelling, changed dashboard layout, added product description
</commit_message>
<xml_diff>
--- a/data/task_status.xlsx
+++ b/data/task_status.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">DPM_3</t>
   </si>
   <si>
-    <t xml:space="preserve">commited</t>
+    <t xml:space="preserve">committed</t>
   </si>
   <si>
     <t xml:space="preserve">67_5</t>
@@ -291,7 +291,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -393,18 +393,18 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>